<commit_message>
Ajout heures de massos, mardi et mercredi
</commit_message>
<xml_diff>
--- a/excel/med_masso.xlsx
+++ b/excel/med_masso.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2023/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABF4B66-06AF-A643-9C84-5F3A823329FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116CE544-726B-F449-8FC2-62ED33509DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="560" windowWidth="34040" windowHeight="28180" activeTab="1" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>code</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>According to availability</t>
+  </si>
+  <si>
+    <t>Après la course - Claudie Germain</t>
+  </si>
+  <si>
+    <t>After the race - Claudie Germain</t>
   </si>
 </sst>
 </file>
@@ -173,7 +179,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Bureau">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -211,7 +217,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Bureau">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -317,7 +323,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Bureau">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -589,7 +595,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,13 +635,11 @@
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="str">
-        <f>B2</f>
-        <v>Selon les diponibilités</v>
-      </c>
-      <c r="C3" s="4" t="str">
-        <f>C2</f>
-        <v>According to availability</v>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -645,24 +649,24 @@
       </c>
       <c r="B4" s="5" t="str">
         <f t="shared" ref="B4:B8" si="0">B3</f>
-        <v>Selon les diponibilités</v>
+        <v>Après la course - Claudie Germain</v>
       </c>
       <c r="C4" s="4" t="str">
         <f>C3</f>
-        <v>According to availability</v>
+        <v>After the race - Claudie Germain</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f>B2</f>
         <v>Selon les diponibilités</v>
       </c>
-      <c r="C5" s="4" t="str">
-        <f>C4</f>
+      <c r="C5" s="5" t="str">
+        <f>C2</f>
         <v>According to availability</v>
       </c>
       <c r="D5" s="3"/>

</xml_diff>